<commit_message>
Fixing typo in tab name
</commit_message>
<xml_diff>
--- a/src/assets/em-seq.xlsx
+++ b/src/assets/em-seq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D578C8A5-F517-6948-87EA-D5B05B94309A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A015FC-A411-E749-8A36-B9AF775957E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{C7B9BE7A-8CF1-DC4E-B597-460D140DCCAC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{C7B9BE7A-8CF1-DC4E-B597-460D140DCCAC}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="run" sheetId="3" r:id="rId3"/>
     <sheet name="experiment ena" sheetId="4" r:id="rId4"/>
     <sheet name="em-seq" sheetId="5" r:id="rId5"/>
-    <sheet name="faang_field_value" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="faang_field_values" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1250,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB1D775-2AD5-3D45-BB1A-353B192F9C79}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1301,7 +1301,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA54AFC2-28E1-2F48-8F7E-981185124EAB}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$19:$O$19</xm:f>
+            <xm:f>faang_field_values!$A$19:$O$19</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -1380,19 +1380,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F06C924-BC48-1E41-96D6-5A29240B33A8}">
           <x14:formula1>
-            <xm:f>faang_field_value!$I$20:$X$20</xm:f>
+            <xm:f>faang_field_values!$I$20:$X$20</xm:f>
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{08FA2A1A-31A0-294C-BEB3-A45B6CB6A92C}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$18:$B$18</xm:f>
+            <xm:f>faang_field_values!$A$18:$B$18</xm:f>
           </x14:formula1>
           <xm:sqref>G2 K2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B208995-E0CC-0049-8E3D-A7A7E5E067A3}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$20:$X$20</xm:f>
+            <xm:f>faang_field_values!$A$20:$X$20</xm:f>
           </x14:formula1>
           <xm:sqref>J2</xm:sqref>
         </x14:dataValidation>
@@ -1483,37 +1483,37 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EABAC30-2C43-3948-94FC-2B81A14E18F9}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$12:$AJ$12</xm:f>
+            <xm:f>faang_field_values!$A$12:$AJ$12</xm:f>
           </x14:formula1>
           <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4CC16AC-8D88-FD48-B96A-99C28DC1EE72}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$13:$I$13</xm:f>
+            <xm:f>faang_field_values!$A$13:$I$13</xm:f>
           </x14:formula1>
           <xm:sqref>H2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2CEFD342-7860-3942-A7EE-532A0985FD60}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$14:$AE$14</xm:f>
+            <xm:f>faang_field_values!$A$14:$AE$14</xm:f>
           </x14:formula1>
           <xm:sqref>I2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D9A05057-3F4C-134B-B92F-3072357AC8B0}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$15:$B$15</xm:f>
+            <xm:f>faang_field_values!$A$15:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>J2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B99DE398-AE87-B54A-8AB6-F9260D9BAE04}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$16:$J$16</xm:f>
+            <xm:f>faang_field_values!$A$16:$J$16</xm:f>
           </x14:formula1>
           <xm:sqref>N2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{871EF185-F5F7-5244-A7E2-D9D2B423C14F}">
           <x14:formula1>
-            <xm:f>faang_field_value!$A$17:$BB$17</xm:f>
+            <xm:f>faang_field_values!$A$17:$BB$17</xm:f>
           </x14:formula1>
           <xm:sqref>O2</xm:sqref>
         </x14:dataValidation>
@@ -1527,7 +1527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034DBD0A-9980-EC4D-95F3-03559F122478}">
   <dimension ref="A1:AF1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3457,7 +3457,7 @@
     <row r="999" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0RBzI267AQ0cpEO0nbPOFiT1/AuKqh1Ou9oG9yEKKQJIUZS+Zc/doo1M+m4P+6YtDFK9d0x8KQUjaiJQ/R46HA==" saltValue="1te7llp2ttNkOJkoEmrpQg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="afyENvfa6ymhtOaB33B/2WeQLIpS12GoksYR9ZMDTI4x2sXhm2y3Tm/E/43y+7DkOslM31yARGeFAm0E8MWJBg==" saltValue="HWDoP6aTZJZ6Yj4Te6oOpw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>